<commit_message>
Aggiorna test_turni.xlsx con nuovi parametri
</commit_message>
<xml_diff>
--- a/test_turni.xlsx
+++ b/test_turni.xlsx
@@ -698,11 +698,7 @@
           <t>Mario Rossi</t>
         </is>
       </c>
-      <c r="D12" s="4" t="inlineStr">
-        <is>
-          <t>Luigi Bianchi</t>
-        </is>
-      </c>
+      <c r="D12" s="4" t="n"/>
       <c r="E12" s="4" t="n"/>
     </row>
     <row r="13">
@@ -854,11 +850,7 @@
           <t>Domenica</t>
         </is>
       </c>
-      <c r="C19" s="4" t="inlineStr">
-        <is>
-          <t>Luigi Bianchi</t>
-        </is>
-      </c>
+      <c r="C19" s="4" t="n"/>
       <c r="D19" s="4" t="inlineStr">
         <is>
           <t>Mario Rossi</t>
@@ -1020,11 +1012,7 @@
           <t>Mario Rossi</t>
         </is>
       </c>
-      <c r="D26" s="4" t="inlineStr">
-        <is>
-          <t>Luigi Bianchi</t>
-        </is>
-      </c>
+      <c r="D26" s="4" t="n"/>
       <c r="E26" s="4" t="n"/>
     </row>
     <row r="27">
@@ -1066,7 +1054,11 @@
           <t>Mario Rossi</t>
         </is>
       </c>
-      <c r="D28" s="3" t="n"/>
+      <c r="D28" s="3" t="inlineStr">
+        <is>
+          <t>Luigi Bianchi</t>
+        </is>
+      </c>
       <c r="E28" s="3" t="n"/>
     </row>
     <row r="29">
@@ -1080,7 +1072,11 @@
           <t>Mercoledì</t>
         </is>
       </c>
-      <c r="C29" s="3" t="n"/>
+      <c r="C29" s="3" t="inlineStr">
+        <is>
+          <t>Luigi Bianchi</t>
+        </is>
+      </c>
       <c r="D29" s="3" t="inlineStr">
         <is>
           <t>Mario Rossi</t>
@@ -1104,7 +1100,11 @@
           <t>Mario Rossi</t>
         </is>
       </c>
-      <c r="D30" s="3" t="n"/>
+      <c r="D30" s="3" t="inlineStr">
+        <is>
+          <t>Luigi Bianchi</t>
+        </is>
+      </c>
       <c r="E30" s="3" t="n"/>
     </row>
     <row r="31">
@@ -1118,8 +1118,16 @@
           <t>Venerdì</t>
         </is>
       </c>
-      <c r="C31" s="3" t="n"/>
-      <c r="D31" s="3" t="n"/>
+      <c r="C31" s="3" t="inlineStr">
+        <is>
+          <t>Luigi Bianchi</t>
+        </is>
+      </c>
+      <c r="D31" s="3" t="inlineStr">
+        <is>
+          <t>Mario Rossi</t>
+        </is>
+      </c>
       <c r="E31" s="3" t="n"/>
     </row>
     <row r="32">
@@ -1133,8 +1141,16 @@
           <t>Sabato</t>
         </is>
       </c>
-      <c r="C32" s="3" t="n"/>
-      <c r="D32" s="3" t="n"/>
+      <c r="C32" s="3" t="inlineStr">
+        <is>
+          <t>Mario Rossi</t>
+        </is>
+      </c>
+      <c r="D32" s="3" t="inlineStr">
+        <is>
+          <t>Luigi Bianchi</t>
+        </is>
+      </c>
       <c r="E32" s="3" t="n"/>
     </row>
     <row r="33">
@@ -1149,7 +1165,11 @@
         </is>
       </c>
       <c r="C33" s="4" t="n"/>
-      <c r="D33" s="4" t="n"/>
+      <c r="D33" s="4" t="inlineStr">
+        <is>
+          <t>Mario Rossi</t>
+        </is>
+      </c>
       <c r="E33" s="4" t="n"/>
     </row>
   </sheetData>
@@ -1228,7 +1248,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>162</v>
+        <v>180</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -1236,7 +1256,7 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6">
@@ -1246,7 +1266,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>144</v>
+        <v>156</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -1254,7 +1274,7 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13">
@@ -1283,7 +1303,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16">
@@ -1293,7 +1313,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1338,12 +1358,12 @@
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>Ore Contratto</t>
+          <t>Ore Contratto (min)</t>
         </is>
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>Ore Max</t>
+          <t>Ore Max (sett)</t>
         </is>
       </c>
       <c r="D3" s="2" t="inlineStr">
@@ -1372,7 +1392,7 @@
         <v>40</v>
       </c>
       <c r="C4" t="n">
-        <v>160</v>
+        <v>45</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -1400,7 +1420,7 @@
         <v>36</v>
       </c>
       <c r="C5" t="n">
-        <v>144</v>
+        <v>40</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>

</xml_diff>